<commit_message>
Changed all Whole Comm to non-Verruco
</commit_message>
<xml_diff>
--- a/tables/bioenv_results.xlsx
+++ b/tables/bioenv_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24420" windowHeight="14220" tabRatio="500"/>
+    <workbookView xWindow="-33720" yWindow="-3740" windowWidth="24420" windowHeight="14220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
   <si>
     <t>Inland (n = 126)</t>
   </si>
@@ -27,21 +27,12 @@
     <t>Verrucomicrobia</t>
   </si>
   <si>
-    <t>Whole Community</t>
-  </si>
-  <si>
     <t>DO</t>
   </si>
   <si>
     <t>0.445 (0.01*)</t>
   </si>
   <si>
-    <t>0.179 (0.01**)</t>
-  </si>
-  <si>
-    <t>0.551 (0.01**)</t>
-  </si>
-  <si>
     <t>PP</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>TKN</t>
   </si>
   <si>
-    <t>0.373 (0.01**)</t>
-  </si>
-  <si>
     <t>Turbidity</t>
   </si>
   <si>
@@ -136,6 +124,18 @@
   </si>
   <si>
     <t>Estuary (n = 44)</t>
+  </si>
+  <si>
+    <t>Non-Verrucomicrobia</t>
+  </si>
+  <si>
+    <t>0.373 (0.02*)</t>
+  </si>
+  <si>
+    <t>0.189 (0.39)</t>
+  </si>
+  <si>
+    <t>0.063 (0.4)</t>
   </si>
 </sst>
 </file>
@@ -335,8 +335,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -459,7 +463,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -486,6 +490,8 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -512,6 +518,8 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -844,7 +852,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -860,11 +868,11 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="39" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="40"/>
       <c r="D1" s="39" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E1" s="40"/>
       <c r="F1" s="39" t="s">
@@ -877,167 +885,167 @@
         <v>1</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>2</v>
+      <c r="G2" s="23" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="14"/>
       <c r="B4" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="14"/>
       <c r="B5" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I5" s="38"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="14"/>
       <c r="B6" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I6" s="38"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="14"/>
       <c r="B7" s="14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I7" s="38"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="14"/>
       <c r="B8" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I8" s="38"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="14"/>
       <c r="B9" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F9" s="34"/>
       <c r="G9" s="30"/>
@@ -1046,16 +1054,16 @@
     <row r="10" spans="1:9">
       <c r="A10" s="14"/>
       <c r="B10" s="14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="30"/>
@@ -1064,16 +1072,16 @@
     <row r="11" spans="1:9">
       <c r="A11" s="14"/>
       <c r="B11" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="30"/>
@@ -1082,16 +1090,16 @@
     <row r="12" spans="1:9">
       <c r="A12" s="14"/>
       <c r="B12" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="30"/>
@@ -1100,16 +1108,16 @@
     <row r="13" spans="1:9">
       <c r="A13" s="14"/>
       <c r="B13" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="30"/>
@@ -1118,16 +1126,16 @@
     <row r="14" spans="1:9">
       <c r="A14" s="14"/>
       <c r="B14" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="30"/>
@@ -1136,16 +1144,16 @@
     <row r="15" spans="1:9">
       <c r="A15" s="14"/>
       <c r="B15" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="30"/>
@@ -1156,10 +1164,10 @@
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F16" s="34"/>
       <c r="G16" s="30"/>
@@ -1170,10 +1178,10 @@
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="30"/>
@@ -1184,10 +1192,10 @@
       <c r="B18" s="15"/>
       <c r="C18" s="14"/>
       <c r="D18" s="15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="31"/>
@@ -1195,25 +1203,25 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>10</v>
-      </c>
       <c r="E19" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I19" s="38"/>
     </row>
@@ -1221,19 +1229,19 @@
       <c r="A20" s="10"/>
       <c r="B20" s="17"/>
       <c r="C20" s="14" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I20" s="38"/>
     </row>
@@ -1241,20 +1249,18 @@
       <c r="A21" s="10"/>
       <c r="B21" s="17"/>
       <c r="C21" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>13</v>
-      </c>
+      <c r="G21" s="14"/>
       <c r="I21" s="38"/>
     </row>
     <row r="22" spans="1:9">
@@ -1264,34 +1270,32 @@
       <c r="D22" s="37"/>
       <c r="E22" s="21"/>
       <c r="F22" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G22" s="15"/>
       <c r="I22" s="38"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D23" s="22">
         <v>0.125</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="I23" s="38"/>
     </row>

</xml_diff>